<commit_message>
initial data manipulation structure commit
</commit_message>
<xml_diff>
--- a/adsb-product-backlog.xlsx
+++ b/adsb-product-backlog.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\adsb-sim-graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB403C0C-6B1C-4420-8C6E-7207D4E2CD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49887C2A-7192-4D60-AE36-096D79AECF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="-Disclaimer-" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$30</definedName>
     <definedName name="Priority">'Agile Product Backlog'!$P$5:$P$7</definedName>
     <definedName name="Status">'Agile Product Backlog'!$Q$5:$Q$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$30</definedName>
     <definedName name="YesNo">'Agile Product Backlog'!$O$5:$O$6</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
@@ -46,15 +46,6 @@
     <t>Sprint 1</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
     <t>Sprint 2</t>
   </si>
   <si>
@@ -170,6 +161,15 @@
   </si>
   <si>
     <t>Emir Alper Yıldız</t>
+  </si>
+  <si>
+    <t>Arayüz Geliştirme 1</t>
+  </si>
+  <si>
+    <t>API 1</t>
+  </si>
+  <si>
+    <t>DataMan 1</t>
   </si>
 </sst>
 </file>
@@ -717,30 +717,30 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="4" customWidth="1"/>
-    <col min="3" max="5" width="33.125" style="4" customWidth="1"/>
-    <col min="6" max="7" width="10.875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="3.3984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.8984375" style="4" customWidth="1"/>
+    <col min="3" max="5" width="33.09765625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="10.8984375" style="4" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.375" style="4" customWidth="1"/>
-    <col min="15" max="17" width="17.875" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.375" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="10.875" style="4"/>
+    <col min="9" max="9" width="13.8984375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.3984375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.59765625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.8984375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.3984375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.3984375" style="4" customWidth="1"/>
+    <col min="15" max="17" width="17.8984375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.3984375" style="4" customWidth="1"/>
+    <col min="19" max="16384" width="10.8984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:35" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -776,42 +776,42 @@
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
-    <row r="2" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -836,7 +836,7 @@
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
     </row>
-    <row r="3" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -873,46 +873,46 @@
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
     </row>
-    <row r="4" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F4" s="8">
         <v>45334</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L4" s="7">
         <v>1</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="13"/>
@@ -935,52 +935,52 @@
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
     </row>
-    <row r="5" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F5" s="8">
         <v>45334</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L5" s="7">
         <v>4</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>13</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -1001,52 +1001,52 @@
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
     </row>
-    <row r="6" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="F6" s="8">
         <v>45334</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L6" s="7">
         <v>1</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="P6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
@@ -1067,11 +1067,11 @@
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
     </row>
-    <row r="7" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
@@ -1085,10 +1085,10 @@
       <c r="N7" s="3"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>15</v>
       </c>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
@@ -1109,7 +1109,7 @@
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
     </row>
-    <row r="8" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1142,7 +1142,7 @@
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
     </row>
-    <row r="9" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1178,7 +1178,7 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
     </row>
-    <row r="10" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1214,11 +1214,11 @@
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
@@ -1252,7 +1252,7 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
     </row>
-    <row r="12" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1288,7 +1288,7 @@
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
     </row>
-    <row r="13" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -1324,7 +1324,7 @@
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
     </row>
-    <row r="14" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1360,11 +1360,11 @@
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
     </row>
-    <row r="15" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
@@ -1398,7 +1398,7 @@
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
     </row>
-    <row r="16" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1434,7 +1434,7 @@
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
     </row>
-    <row r="17" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1470,7 +1470,7 @@
       <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
     </row>
-    <row r="18" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1506,11 +1506,11 @@
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>
@@ -1544,7 +1544,7 @@
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1580,7 +1580,7 @@
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1616,7 +1616,7 @@
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1652,11 +1652,11 @@
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
@@ -1690,7 +1690,7 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
     </row>
-    <row r="24" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1726,7 +1726,7 @@
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1762,7 +1762,7 @@
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1798,11 +1798,11 @@
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
-    <row r="27" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="6"/>
@@ -1836,7 +1836,7 @@
       <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
     </row>
-    <row r="28" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1872,7 +1872,7 @@
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1908,7 +1908,7 @@
       <c r="AH29" s="3"/>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:35" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1944,7 +1944,7 @@
       <c r="AH30" s="3"/>
       <c r="AI30" s="3"/>
     </row>
-    <row r="31" spans="2:35" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:35" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1979,7 +1979,7 @@
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
     </row>
-    <row r="32" spans="2:35" s="11" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:35" s="11" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2015,7 +2015,7 @@
       <c r="AH32" s="10"/>
       <c r="AI32" s="10"/>
     </row>
-    <row r="33" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -2050,7 +2050,7 @@
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
     </row>
-    <row r="34" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -2085,7 +2085,7 @@
       <c r="AH34" s="3"/>
       <c r="AI34" s="3"/>
     </row>
-    <row r="35" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -2120,7 +2120,7 @@
       <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
     </row>
-    <row r="36" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -2155,7 +2155,7 @@
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
     </row>
-    <row r="37" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -2190,7 +2190,7 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
     </row>
-    <row r="38" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -2225,7 +2225,7 @@
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
     </row>
-    <row r="39" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -2260,7 +2260,7 @@
       <c r="AH39" s="3"/>
       <c r="AI39" s="3"/>
     </row>
-    <row r="40" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -2295,7 +2295,7 @@
       <c r="AH40" s="3"/>
       <c r="AI40" s="3"/>
     </row>
-    <row r="41" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -2330,7 +2330,7 @@
       <c r="AH41" s="3"/>
       <c r="AI41" s="3"/>
     </row>
-    <row r="42" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -2365,7 +2365,7 @@
       <c r="AH42" s="3"/>
       <c r="AI42" s="3"/>
     </row>
-    <row r="43" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -2400,7 +2400,7 @@
       <c r="AH43" s="3"/>
       <c r="AI43" s="3"/>
     </row>
-    <row r="44" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -2435,7 +2435,7 @@
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
     </row>
-    <row r="45" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -2470,7 +2470,7 @@
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
     </row>
-    <row r="46" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -2505,7 +2505,7 @@
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
     </row>
-    <row r="47" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -2540,7 +2540,7 @@
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
     </row>
-    <row r="48" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -2575,7 +2575,7 @@
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
     </row>
-    <row r="49" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -2610,7 +2610,7 @@
       <c r="AH49" s="3"/>
       <c r="AI49" s="3"/>
     </row>
-    <row r="50" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -2645,7 +2645,7 @@
       <c r="AH50" s="3"/>
       <c r="AI50" s="3"/>
     </row>
-    <row r="51" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -2680,7 +2680,7 @@
       <c r="AH51" s="3"/>
       <c r="AI51" s="3"/>
     </row>
-    <row r="52" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -2715,7 +2715,7 @@
       <c r="AH52" s="3"/>
       <c r="AI52" s="3"/>
     </row>
-    <row r="53" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -2750,7 +2750,7 @@
       <c r="AH53" s="3"/>
       <c r="AI53" s="3"/>
     </row>
-    <row r="54" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -2785,7 +2785,7 @@
       <c r="AH54" s="3"/>
       <c r="AI54" s="3"/>
     </row>
-    <row r="55" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -2820,7 +2820,7 @@
       <c r="AH55" s="3"/>
       <c r="AI55" s="3"/>
     </row>
-    <row r="56" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -2855,7 +2855,7 @@
       <c r="AH56" s="3"/>
       <c r="AI56" s="3"/>
     </row>
-    <row r="57" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -2890,7 +2890,7 @@
       <c r="AH57" s="3"/>
       <c r="AI57" s="3"/>
     </row>
-    <row r="58" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -2925,7 +2925,7 @@
       <c r="AH58" s="3"/>
       <c r="AI58" s="3"/>
     </row>
-    <row r="59" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -2960,7 +2960,7 @@
       <c r="AH59" s="3"/>
       <c r="AI59" s="3"/>
     </row>
-    <row r="60" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -2995,7 +2995,7 @@
       <c r="AH60" s="3"/>
       <c r="AI60" s="3"/>
     </row>
-    <row r="61" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -3030,7 +3030,7 @@
       <c r="AH61" s="3"/>
       <c r="AI61" s="3"/>
     </row>
-    <row r="62" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -3065,7 +3065,7 @@
       <c r="AH62" s="3"/>
       <c r="AI62" s="3"/>
     </row>
-    <row r="63" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -3100,7 +3100,7 @@
       <c r="AH63" s="3"/>
       <c r="AI63" s="3"/>
     </row>
-    <row r="64" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -3135,7 +3135,7 @@
       <c r="AH64" s="3"/>
       <c r="AI64" s="3"/>
     </row>
-    <row r="65" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -3170,7 +3170,7 @@
       <c r="AH65" s="3"/>
       <c r="AI65" s="3"/>
     </row>
-    <row r="66" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -3205,7 +3205,7 @@
       <c r="AH66" s="3"/>
       <c r="AI66" s="3"/>
     </row>
-    <row r="67" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -3240,7 +3240,7 @@
       <c r="AH67" s="3"/>
       <c r="AI67" s="3"/>
     </row>
-    <row r="68" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -3275,7 +3275,7 @@
       <c r="AH68" s="3"/>
       <c r="AI68" s="3"/>
     </row>
-    <row r="69" spans="3:35" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:35" x14ac:dyDescent="0.3">
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
@@ -3335,16 +3335,16 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="88.375" style="15" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="15"/>
+    <col min="1" max="1" width="3.3984375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="88.3984375" style="15" customWidth="1"/>
+    <col min="3" max="16384" width="10.8984375" style="15"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>